<commit_message>
Issue 47280: LKSM: Trailing whitespace in Source name won't resolve when deriving samples
</commit_message>
<xml_diff>
--- a/experiment/test/sampledata/sampleType.xlsx
+++ b/experiment/test/sampledata/sampleType.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26004"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10313"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xingyang/dev/trunk/server/modules/platform/experiment/test/sampledata/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3654362D-8BCF-5944-B70B-B53D0C139A40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="640" yWindow="640" windowWidth="27500" windowHeight="12460"/>
+    <workbookView xWindow="640" yWindow="640" windowWidth="27500" windowHeight="12460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -19,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>IntCol</t>
   </si>
@@ -33,15 +39,6 @@
     <t>BoolCol</t>
   </si>
   <si>
-    <t>SampleSetBVT1</t>
-  </si>
-  <si>
-    <t>a</t>
-  </si>
-  <si>
-    <t>SampleSetBVT2</t>
-  </si>
-  <si>
     <t>b</t>
   </si>
   <si>
@@ -61,12 +58,24 @@
   </si>
   <si>
     <t>Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SampleSetBVT1  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">a </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SampleSetBVT2   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">TRUE </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -131,10 +140,10 @@
     <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
@@ -146,6 +155,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -437,16 +449,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" customHeight="1">
+    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -461,35 +475,35 @@
         <v>3</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.75" customHeight="1">
+    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="B2" s="1">
         <v>100</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="D2" s="2">
         <v>36526</v>
       </c>
-      <c r="E2" s="1" t="b">
-        <v>1</v>
+      <c r="E2" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15.75" customHeight="1">
+    <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="B3" s="1">
         <v>200</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D3" s="2">
         <v>36558</v>
@@ -498,15 +512,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15.75" customHeight="1">
+    <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B4" s="1">
         <v>300</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D4" s="2">
         <v>36588</v>
@@ -515,15 +529,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="15.75" customHeight="1">
+    <row r="5" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B5" s="1">
         <v>400</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D5" s="2">
         <v>36620</v>

</xml_diff>

<commit_message>
Issue 47280: LKSM: Trailing whitespace in Source name won't resolve when deriving samples (#4150)
</commit_message>
<xml_diff>
--- a/experiment/test/sampledata/sampleType.xlsx
+++ b/experiment/test/sampledata/sampleType.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26004"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10313"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xingyang/dev/trunk/server/modules/platform/experiment/test/sampledata/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A37DC57-96D8-E846-A018-BF89F01B020B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="640" yWindow="640" windowWidth="27500" windowHeight="12460"/>
+    <workbookView xWindow="640" yWindow="640" windowWidth="27500" windowHeight="12460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -33,15 +39,6 @@
     <t>BoolCol</t>
   </si>
   <si>
-    <t>SampleSetBVT1</t>
-  </si>
-  <si>
-    <t>a</t>
-  </si>
-  <si>
-    <t>SampleSetBVT2</t>
-  </si>
-  <si>
     <t>b</t>
   </si>
   <si>
@@ -61,12 +58,21 @@
   </si>
   <si>
     <t>Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SampleSetBVT1  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">a </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SampleSetBVT2   </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -131,10 +137,10 @@
     <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
@@ -146,6 +152,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -437,16 +446,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" customHeight="1">
+    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -461,18 +472,18 @@
         <v>3</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.75" customHeight="1">
+    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="B2" s="1">
         <v>100</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="D2" s="2">
         <v>36526</v>
@@ -481,15 +492,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15.75" customHeight="1">
+    <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="B3" s="1">
         <v>200</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D3" s="2">
         <v>36558</v>
@@ -498,15 +509,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15.75" customHeight="1">
+    <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B4" s="1">
         <v>300</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D4" s="2">
         <v>36588</v>
@@ -515,15 +526,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="15.75" customHeight="1">
+    <row r="5" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B5" s="1">
         <v>400</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D5" s="2">
         <v>36620</v>

</xml_diff>